<commit_message>
Web Deployment Ver 1.0
Updated Shiny App for web deployment and test datasets with realistic data. Updated calculation to correct formula
</commit_message>
<xml_diff>
--- a/PondCalCompleted.xlsx
+++ b/PondCalCompleted.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Risato\Desktop\Gdrive-WBUG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RisatoMob\Documents\GitHub\PondCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C198E73-A8C9-4D5D-A495-74D0177FA635}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Depth</t>
   </si>
@@ -37,12 +38,21 @@
   <si>
     <t>IslandDepth</t>
   </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Island Volume</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,16 +60,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -67,12 +99,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,102 +448,169 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>34532</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
         <v>2345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>234562</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2790</v>
+      </c>
+      <c r="C3">
+        <f>(A3-A2)*(B3+B2)/2</f>
+        <v>1395</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>432</v>
+      </c>
+      <c r="G3">
+        <f>(E3-E2)*(F3+F2)/2</f>
+        <v>1388.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>45321</v>
+      <c r="B4" s="1">
+        <v>6000</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+        <f t="shared" ref="C4:C7" si="0">(A4-A3)*(B4+B3)/2</f>
+        <v>4395</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>46</v>
+      </c>
+      <c r="G4">
+        <f>(E4-E3)*(F4+F3)/2</f>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12000</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>16000</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>78902</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>109822</v>
-      </c>
-      <c r="D6">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>45</v>
-      </c>
-      <c r="B7">
-        <v>345621</v>
+      <c r="B7" s="1">
+        <v>30492</v>
       </c>
       <c r="C7">
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>25246</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUM(C3:C7)/43560</f>
+        <v>1.2864095500459136</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2">
+        <f>SUM(G2:G7)/43560</f>
+        <v>4.2848943985307621E-2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="4">
+        <f>C9-G9</f>
+        <v>1.2435606060606059</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="F2:F7">
+    <sortCondition ref="F2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>